<commit_message>
se terminó el manuel tecnico y se actualizaron algunos diagramas con el script de la base de datos
</commit_message>
<xml_diff>
--- a/BasesDeDatos/DD_ViveRegistro.xlsx
+++ b/BasesDeDatos/DD_ViveRegistro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeison\Desktop\ViveRegistro-Sistema\ViveRegistro\documentacion\BasesDeDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66C2590-F30E-458D-8B40-933AAF5D736D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FD7B6D-D4EB-4979-A346-C7FA37662BD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="96">
   <si>
     <t>Nota: Los campos en negrita son la clave primaria  y Foranea de las tablas.</t>
   </si>
@@ -188,6 +188,132 @@
   <si>
     <t>Diccionario de datos: ViveRegistro</t>
   </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada sensor de humedad</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave foranea de la tabla, la cual sirve para intercambiar datos con la tabla "plantas" y relacionar cada sensor con cada una de las tablas que se encuentren registradas en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará un valor por defecto dependiendo del sensor, en este caso, guardará el valor de "Humedad", ya que es el tipo de sensor que representa al sensor de humedad</t>
+  </si>
+  <si>
+    <t>Este campo guardará una serie de strings que representaran el color de cada sensor en relación a las graficas del sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará la fecha en la cual se creé un nuevo registro en esta tabla, o sea, cuando se cree un nuevo sensor de humedad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este campo sirve para almacenar el nombre de cada sensor de humedad </t>
+  </si>
+  <si>
+    <t>Este campo guardará la fecha en la cual se cree un nuevo registro en esta tabla, o sea, cuando se cree un nuevo sensor de temperatura</t>
+  </si>
+  <si>
+    <t>Este campo guardará el nombre de cada sensor de temperatura</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada planta que exista en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada sensor de temperatura que existe en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará el nombre que se le asigne a cada planta del sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará una breve descripción de la planta, desde sus caracteristicas basicas como principales</t>
+  </si>
+  <si>
+    <t>Este campo guardará un valor por defecto dependiendo del sensor, en este caso, guardará el valor de "temperatura", ya que es el tipo de sensor que representa al sensor de temperatura</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada sensor de lluvia que exista en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará el porcentaje de lluvia que sea enviado desde el sensor de lluvia</t>
+  </si>
+  <si>
+    <t>Este campo guardará el estado del sensor, si está apagado o prendido</t>
+  </si>
+  <si>
+    <t>Este campo guardará la descripción de la lluvia, o sea, si es muy fuerte, mediana o nula</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada usuario registrado en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará el nombre de usuario que tenga el usuario en su correo, o sea, solo se guardará cuando el usuario se logueé por modalidad de "Logueo por medio de Google"</t>
+  </si>
+  <si>
+    <t>Este campo guardará el correo con el cual se registre el usuario al sistema, el cual servirá para cosas como reestablecer la contraseña, etc.</t>
+  </si>
+  <si>
+    <t>Este campo guardará el estado de verificación del usuario, o sea, guardará un booleano, el cual pasará a ser verdadero cuando el usuario haya hecho la verificación despues de registrarse con su correo en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará la contraseña con la cual el usuario se registre en el sistema, esta la podrá usar el mismo usuario para loguearse en el sistema</t>
+  </si>
+  <si>
+    <t>Este campo guardará el estado en el que se encuentre el usuario, si en estado activo o inactivo</t>
+  </si>
+  <si>
+    <t>Este campo guardará la URL de la foto del usuario cuando este, se logue por medio de google, en caso contrario, no se guardará nada en este campo, o sea que, permite nulos</t>
+  </si>
+  <si>
+    <t>Este campo guardará el role del usuario, donde solo existiran dos tipos de role, usuario y administrador</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada registro que venga de los sensores de humedad</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave foranea de la tabla, en la cual se guardará el id del sensor de humedad al cual le corresponda el registro de humedad</t>
+  </si>
+  <si>
+    <t>Este campo guardará el porcentaje de humedad que se calcule por medio de validaciones que se le hace a los datos que proveen los sensores de humedad</t>
+  </si>
+  <si>
+    <t>Este campo guardará el estado del sensor de humedad correspondiente al registro de humedad que se haga, o sea, si se encuentra prendido o apagado</t>
+  </si>
+  <si>
+    <t>Este campo guardará una breve descripción de la humedad de la planta, si es muy alta, media, baja o nula</t>
+  </si>
+  <si>
+    <t>Este campo guardará una breve descripción de la temperatura del ambiente donde se encuentre el sensor de temperatura, o sea,  si es muy alta, media, baja o nula</t>
+  </si>
+  <si>
+    <t>Este campo guardará el estado del sensor de temperatura correspondiente al registro de temperatura que se haga, o sea, si se encuentra prendido o apagado</t>
+  </si>
+  <si>
+    <t>Este campo guardará la temperatura en grados celsius que se calcule por medio de validaciones que se le hace a los datos que proveen los sensores de temperatura</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave primaria de la tabla, la cual sirve de identificador para cada registro que venga de los sensores de temperatura</t>
+  </si>
+  <si>
+    <t>Este campo representa la clave foranea de la tabla, en la cual se guardará el id del sensor de temperatura al cual le corresponda el registro de temperatura</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de almacenar los registros correspondientes de cada una de las plantas que se creen en el sistema, donde tendrá su identificador principal, y datos que permita diferenciar cada una de las plantas</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de guardar cada uno de los usuarios que se registren en el sistema, donde cada uno tendrá su propio identificador, contraseña y email, los cuales usaran para poder loguerase y autenticarse en el sistema</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de guardar los registros correspondientes de cada uno de los sensores de lluvia que se creen en el sistema, ademas, se podran hacer todo tipo de operaciones y consultas desde y a esta tabla, donde cada sensor tendrá su identificador y datos que lo caractericen</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de guardar y crear un historico de todos los registros que se envien desde los sensores de humedad, para poder graficarlos y generar informes</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de guardar y crear un historico de todos los registros que se envien desde los sensores de temperatura, para poder graficarlos y generar informes</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de guardar los registros correspondientes de cada uno de los sensores de humedad que se creen en el sistema, ademas, se podran hacer todo tipo de operaciones y consultas desde y a esta tabla, donde cada sensor tendrá su identificador y datos que lo caractericen</t>
+  </si>
+  <si>
+    <t>Esta tabla se encargará de guardar los registros correspondientes de cada uno de los sensores de temperatura que se creen en el sistema, ademas, se podran hacer todo tipo de operaciones y consultas desde y a esta tabla, donde cada sensor tendrá su identificador y datos que lo caractericen</t>
+  </si>
 </sst>
 </file>
 
@@ -289,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -357,26 +483,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -395,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -436,34 +542,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -475,6 +569,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -484,23 +587,192 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="43">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -792,64 +1064,64 @@
   </dxfs>
   <tableStyles count="12">
     <tableStyle name="Hoja1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="firstRowStripe" dxfId="34"/>
-      <tableStyleElement type="secondRowStripe" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
+      <tableStyleElement type="firstRowStripe" dxfId="41"/>
+      <tableStyleElement type="secondRowStripe" dxfId="40"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="32"/>
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="secondRowStripe" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="39"/>
+      <tableStyleElement type="firstRowStripe" dxfId="38"/>
+      <tableStyleElement type="secondRowStripe" dxfId="37"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="29"/>
-      <tableStyleElement type="firstRowStripe" dxfId="28"/>
-      <tableStyleElement type="secondRowStripe" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+      <tableStyleElement type="secondRowStripe" dxfId="34"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="firstRowStripe" dxfId="25"/>
-      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="23"/>
-      <tableStyleElement type="firstRowStripe" dxfId="22"/>
-      <tableStyleElement type="secondRowStripe" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="29"/>
+      <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="firstRowStripe" dxfId="26"/>
+      <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
-      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="firstRowStripe" dxfId="23"/>
+      <tableStyleElement type="secondRowStripe" dxfId="22"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="firstRowStripe" dxfId="13"/>
-      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="firstRowStripe" dxfId="20"/>
+      <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 9" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="secondRowStripe" dxfId="16"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 10" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="secondRowStripe" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 11" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0A000000}">
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="Hoja1-style 12" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0B000000}">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -877,13 +1149,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_9" displayName="Table_9" ref="A46:E54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_9" displayName="Table_9" ref="A46:E54" headerRowDxfId="1" totalsRowDxfId="0">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Campo"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Tipo"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="nulos"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Identidad"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Descripción"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Campo" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Tipo" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="nulos" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Identidad" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Descripción" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style 9" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1154,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1170,13 +1442,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1199,13 +1471,13 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1285,12 +1557,12 @@
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1312,14 +1584,16 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="B6" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1391,7 +1665,9 @@
       <c r="D8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1413,8 +1689,8 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1426,7 +1702,9 @@
       <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1452,7 +1730,7 @@
       <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1461,7 +1739,9 @@
       <c r="D10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1483,11 +1763,11 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1496,7 +1776,9 @@
       <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1522,7 +1804,7 @@
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1531,7 +1813,9 @@
       <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1557,7 +1841,7 @@
       <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1566,7 +1850,9 @@
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1636,12 +1922,12 @@
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1667,10 +1953,12 @@
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="B17" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1730,7 +2018,7 @@
       <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -1742,7 +2030,9 @@
       <c r="D19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1764,8 +2054,8 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1777,7 +2067,9 @@
       <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1800,10 +2092,10 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -1812,7 +2104,9 @@
       <c r="D21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1834,11 +2128,11 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+    <row r="22" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -1847,7 +2141,9 @@
       <c r="D22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1870,10 +2166,10 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -1882,7 +2178,9 @@
       <c r="D23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1904,11 +2202,11 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -1917,7 +2215,9 @@
       <c r="D24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="10"/>
+      <c r="E24" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1992,12 +2292,12 @@
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2023,10 +2323,12 @@
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
+      <c r="B28" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2086,10 +2388,10 @@
       <c r="Y29" s="1"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -2098,7 +2400,9 @@
       <c r="D30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2121,10 +2425,10 @@
       <c r="Y30" s="1"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -2133,7 +2437,9 @@
       <c r="D31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2156,10 +2462,10 @@
       <c r="Y31" s="1"/>
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -2168,7 +2474,9 @@
       <c r="D32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2248,12 +2556,12 @@
       <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="29"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2275,14 +2583,16 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
     </row>
-    <row r="36" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19"/>
+      <c r="B36" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2354,7 +2664,9 @@
       <c r="D38" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2376,7 +2688,7 @@
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
     </row>
-    <row r="39" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>22</v>
       </c>
@@ -2389,7 +2701,9 @@
       <c r="D39" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2424,7 +2738,9 @@
       <c r="D40" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2459,7 +2775,9 @@
       <c r="D41" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2536,15 +2854,15 @@
       <c r="Y43" s="1"/>
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2566,14 +2884,16 @@
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
     </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="19"/>
+      <c r="B45" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2596,19 +2916,19 @@
       <c r="Y45" s="1"/>
     </row>
     <row r="46" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="38" t="s">
         <v>2</v>
       </c>
       <c r="F46" s="1"/>
@@ -2633,19 +2953,21 @@
       <c r="Y46" s="1"/>
     </row>
     <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2667,20 +2989,22 @@
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2702,20 +3026,22 @@
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+    <row r="49" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="7"/>
+      <c r="E49" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -2737,20 +3063,22 @@
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
     </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2772,20 +3100,22 @@
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
     </row>
-    <row r="51" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+    <row r="51" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="7"/>
+      <c r="E51" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2808,19 +3138,21 @@
       <c r="Y51" s="1"/>
     </row>
     <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="7"/>
+      <c r="E52" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2842,20 +3174,22 @@
       <c r="X52" s="1"/>
       <c r="Y52" s="1"/>
     </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="s">
+    <row r="53" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="20"/>
+      <c r="E53" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -2878,19 +3212,21 @@
       <c r="Y53" s="1"/>
     </row>
     <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="21" t="s">
+      <c r="D54" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="21"/>
+      <c r="E54" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2943,12 +3279,12 @@
       <c r="A56" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="26"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="22"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -2974,10 +3310,12 @@
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="26"/>
+      <c r="B57" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="34"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -3036,8 +3374,8 @@
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
     </row>
-    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30" t="s">
+    <row r="59" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="12" t="s">
@@ -3049,7 +3387,9 @@
       <c r="D59" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="12"/>
+      <c r="E59" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -3071,8 +3411,8 @@
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
     </row>
-    <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="22" t="s">
+    <row r="60" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -3084,7 +3424,9 @@
       <c r="D60" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -3106,11 +3448,11 @@
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
     </row>
-    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
+    <row r="61" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="10" t="s">
@@ -3119,7 +3461,9 @@
       <c r="D61" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E61" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -3141,11 +3485,11 @@
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
     </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="23" t="s">
+    <row r="62" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="10" t="s">
@@ -3154,7 +3498,9 @@
       <c r="D62" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="10"/>
+      <c r="E62" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -3177,10 +3523,10 @@
       <c r="Y62" s="1"/>
     </row>
     <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="23" t="s">
+      <c r="B63" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="10" t="s">
@@ -3189,7 +3535,9 @@
       <c r="D63" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="10"/>
+      <c r="E63" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -3269,12 +3617,12 @@
       <c r="A66" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B66" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="26"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="22"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -3300,10 +3648,12 @@
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="24"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="26"/>
+      <c r="B67" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="34"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -3362,8 +3712,8 @@
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
     </row>
-    <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="30" t="s">
+    <row r="69" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
         <v>49</v>
       </c>
       <c r="B69" s="12" t="s">
@@ -3375,7 +3725,9 @@
       <c r="D69" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="12"/>
+      <c r="E69" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3397,8 +3749,8 @@
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
     </row>
-    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="22" t="s">
+    <row r="70" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -3410,7 +3762,9 @@
       <c r="D70" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="8"/>
+      <c r="E70" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3432,11 +3786,11 @@
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
     </row>
-    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="23" t="s">
+    <row r="71" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="10" t="s">
@@ -3445,7 +3799,9 @@
       <c r="D71" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="10"/>
+      <c r="E71" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -3467,11 +3823,11 @@
       <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
     </row>
-    <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="23" t="s">
+    <row r="72" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B72" s="23" t="s">
+      <c r="B72" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C72" s="10" t="s">
@@ -3480,7 +3836,9 @@
       <c r="D72" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="10"/>
+      <c r="E72" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -3502,11 +3860,11 @@
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
     </row>
-    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="23" t="s">
+    <row r="73" spans="1:25" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C73" s="10" t="s">
@@ -3515,7 +3873,9 @@
       <c r="D73" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="10"/>
+      <c r="E73" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>

</xml_diff>